<commit_message>
Add Function Dependency FNAME, APMT -> APMT
</commit_message>
<xml_diff>
--- a/input/Truth-easy-compare.xlsx
+++ b/input/Truth-easy-compare.xlsx
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152:G155"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C78" sqref="A78:C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -2245,13 +2245,13 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A78" s="2">
+      <c r="A78" s="4">
         <v>30792</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C78" s="2" t="s">
+      <c r="B78" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D78" s="1">
@@ -2345,13 +2345,13 @@
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A83" s="2">
+      <c r="A83" s="4">
         <v>31313</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C83" s="2" t="s">
+      <c r="B83" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C83" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D83" s="1">
@@ -2436,13 +2436,13 @@
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A88" s="2">
+      <c r="A88" s="4">
         <v>31779</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="2">
+      <c r="B88" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="4">
         <v>95825</v>
       </c>
       <c r="D88" s="1">
@@ -2505,13 +2505,13 @@
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A92" s="2">
+      <c r="A92" s="4">
         <v>31981</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="2">
+      <c r="B92" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="4">
         <v>58783</v>
       </c>
       <c r="D92" s="1">
@@ -2547,13 +2547,13 @@
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A95" s="2">
+      <c r="A95" s="4">
         <v>32213</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C95" s="2" t="s">
+      <c r="B95" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D95" s="1">
@@ -2594,13 +2594,13 @@
       <c r="K96" s="1"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A97" s="2">
+      <c r="A97" s="4">
         <v>32466</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="2">
+      <c r="B97" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" s="4">
         <v>37644</v>
       </c>
       <c r="D97" s="1">
@@ -2645,13 +2645,13 @@
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A100" s="2">
+      <c r="A100" s="4">
         <v>32916</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" s="2">
+      <c r="B100" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="4">
         <v>38577</v>
       </c>
       <c r="D100" s="1">
@@ -2765,13 +2765,13 @@
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A107" s="2">
+      <c r="A107" s="4">
         <v>34374</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" s="2">
+      <c r="B107" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" s="4">
         <v>4733</v>
       </c>
       <c r="D107" s="1">
@@ -2876,13 +2876,13 @@
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A113" s="2">
+      <c r="A113" s="4">
         <v>35232</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C113" s="2" t="s">
+      <c r="B113" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C113" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D113" s="1">
@@ -2985,13 +2985,13 @@
       <c r="K118" s="1"/>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A119" s="2">
+      <c r="A119" s="4">
         <v>36279</v>
       </c>
-      <c r="B119" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C119" s="2">
+      <c r="B119" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119" s="4">
         <v>27416</v>
       </c>
       <c r="D119" s="1">
@@ -3122,13 +3122,13 @@
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A129" s="2">
+      <c r="A129" s="4">
         <v>37398</v>
       </c>
-      <c r="B129" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C129" s="2">
+      <c r="B129" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C129" s="4">
         <v>72059</v>
       </c>
       <c r="D129" s="1">
@@ -3231,13 +3231,13 @@
       <c r="J134" s="1"/>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A135" s="2">
+      <c r="A135" s="4">
         <v>38070</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C135" s="2">
+      <c r="B135" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C135" s="4">
         <v>67870</v>
       </c>
       <c r="D135" s="1">
@@ -3251,13 +3251,13 @@
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A136" s="2">
+      <c r="A136" s="4">
         <v>38167</v>
       </c>
-      <c r="B136" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C136" s="2" t="s">
+      <c r="B136" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C136" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D136" s="1">
@@ -3353,13 +3353,13 @@
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A142" s="2">
+      <c r="A142" s="4">
         <v>38552</v>
       </c>
-      <c r="B142" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C142" s="2" t="s">
+      <c r="B142" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C142" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D142" s="1">
@@ -3373,13 +3373,13 @@
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A143" s="2">
+      <c r="A143" s="4">
         <v>38652</v>
       </c>
-      <c r="B143" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C143" s="2" t="s">
+      <c r="B143" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C143" s="4" t="s">
         <v>66</v>
       </c>
       <c r="D143" s="1">
@@ -3453,13 +3453,13 @@
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A147" s="2">
+      <c r="A147" s="4">
         <v>39154</v>
       </c>
-      <c r="B147" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C147" s="2">
+      <c r="B147" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147" s="4">
         <v>80922</v>
       </c>
       <c r="D147" s="1">
@@ -3473,13 +3473,13 @@
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A148" s="2">
+      <c r="A148" s="4">
         <v>39190</v>
       </c>
-      <c r="B148" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C148" s="2" t="s">
+      <c r="B148" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C148" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D148" s="1">
@@ -3493,13 +3493,13 @@
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A149" s="2">
+      <c r="A149" s="4">
         <v>39257</v>
       </c>
-      <c r="B149" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C149" s="2" t="s">
+      <c r="B149" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C149" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D149" s="1">
@@ -3565,13 +3565,13 @@
       <c r="I152" s="1"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A153" s="2">
+      <c r="A153" s="4">
         <v>39835</v>
       </c>
-      <c r="B153" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C153" s="2" t="s">
+      <c r="B153" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C153" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D153" s="1">
@@ -3586,13 +3586,13 @@
       <c r="I153" s="1"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A154" s="2">
+      <c r="A154" s="4">
         <v>39853</v>
       </c>
-      <c r="B154" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C154" s="2">
+      <c r="B154" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C154" s="4">
         <v>50551</v>
       </c>
       <c r="D154" s="1">

</xml_diff>